<commit_message>
ajout dictionnaire au format pdf
</commit_message>
<xml_diff>
--- a/2_dictionnaire/dictionnaire_de_donnees_022026.xlsx
+++ b/2_dictionnaire/dictionnaire_de_donnees_022026.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\compt\Desktop\0_0_0_Foramation_Data_Analyst\0_0_OpenClassRooms\1_Projets\Projet_N5_Créez et utilisez une base de données immobilière avec SQL\A faire\1_Dictionnaire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\compt\Desktop\0_0_0_Foramation_Data_Analyst\Porte_folio_Data_GitHub\nb_p4_Créez et utilisez une base de données immobilière avec SQL\2_dictionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00262B62-D1A8-4088-92C7-033B063FA1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8ED161-1E9A-49EB-88F6-805E8847E106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C7FD492F-4C99-42B6-83AC-AFB79D4413A6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="108">
   <si>
     <t>Type SQL</t>
   </si>
@@ -435,12 +435,15 @@
   <si>
     <t>€</t>
   </si>
+  <si>
+    <t>Dictionnaire des données (phase conception)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,6 +495,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -590,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -639,6 +650,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -974,644 +988,651 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7239D97B-677E-4CE3-976C-E7DFFA9380B4}">
-  <dimension ref="B1:G41"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E2" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.109375" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="39.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="2:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="2" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+    <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
+    <row r="8" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="2" t="s">
+      <c r="E10" s="10"/>
+      <c r="F10" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
+    <row r="11" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="2" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+    <row r="12" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="2" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="7" t="s">
+    <row r="14" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+    <row r="16" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+    <row r="17" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="2" t="s">
+      <c r="E17" s="4"/>
+      <c r="F17" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
+    <row r="18" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
+      <c r="E18" s="4"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="2" t="s">
+      <c r="E19" s="4"/>
+      <c r="F19" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10" t="s">
+    <row r="20" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="2" t="s">
+      <c r="E20" s="4"/>
+      <c r="F20" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="7" t="s">
+    <row r="23" spans="1:6" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="2:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="5" t="s">
+    <row r="25" spans="1:6" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5" t="s">
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="5" t="s">
+    <row r="26" spans="1:6" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="1" t="s">
+      <c r="E26" s="5"/>
+      <c r="F26" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="5" t="s">
+    <row r="27" spans="1:6" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="1" t="s">
+      <c r="E27" s="5"/>
+      <c r="F27" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="5" t="s">
+    <row r="28" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="1" t="s">
+      <c r="E28" s="5"/>
+      <c r="F28" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="5" t="s">
+    <row r="29" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="1" t="s">
+      <c r="E29" s="5"/>
+      <c r="F29" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="5" t="s">
+    <row r="30" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="1" t="s">
+      <c r="E30" s="5"/>
+      <c r="F30" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="5" t="s">
+    <row r="31" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="E31" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="5" t="s">
+    <row r="32" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="E32" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="5" t="s">
+    <row r="33" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="1" t="s">
+      <c r="E33" s="5"/>
+      <c r="F33" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="8" t="s">
+    <row r="34" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="9" t="s">
+      <c r="E34" s="5"/>
+      <c r="F34" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="7" t="s">
+    <row r="36" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="7"/>
-    </row>
-    <row r="35" spans="2:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
+    <row r="38" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4" t="s">
+      <c r="E38" s="4"/>
+      <c r="F38" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
+    <row r="39" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="2" t="s">
+      <c r="E39" s="4"/>
+      <c r="F39" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
+    <row r="40" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="E40" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="4" t="s">
+    <row r="41" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="D41" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="2" t="s">
+      <c r="E41" s="4"/>
+      <c r="F41" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="10" t="s">
+    <row r="42" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="D42" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4" t="s">
+      <c r="E42" s="4"/>
+      <c r="F42" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="11" t="s">
+    <row r="43" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="B43" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="16"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="B43:F43"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="93" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>